<commit_message>
Fix names on Excel and image
</commit_message>
<xml_diff>
--- a/2021/docs/es/assets/Top10Mapping-es.xlsx
+++ b/2021/docs/es/assets/Top10Mapping-es.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmarsicano/git/OWASP/Top10/2021/docs/assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinmarsicano/Git/OWASP/Top10/2021/docs/es/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58290279-ABF0-2442-AD6C-DB3F4BF30D48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164BF1B9-FBB5-1649-843D-266001A78B0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="23500" xr2:uid="{C7D86A64-EE22-7643-AE64-D299E066CB54}"/>
+    <workbookView xWindow="-6080" yWindow="-21100" windowWidth="25600" windowHeight="21100" xr2:uid="{C7D86A64-EE22-7643-AE64-D299E066CB54}"/>
   </bookViews>
   <sheets>
     <sheet name="Top 10 Mapping" sheetId="1" r:id="rId1"/>
@@ -78,28 +78,28 @@
     <t>A03:2021-Inyección</t>
   </si>
   <si>
-    <t>A05:2021-Configuración Incorrecta de Seguridad</t>
-  </si>
-  <si>
-    <t>A04:2021-Diseño Inseguro</t>
-  </si>
-  <si>
-    <t>A02:2021-Fallos Criptográficos</t>
-  </si>
-  <si>
     <t>A06:2021-Componentes Vulnerables y Obsoletos</t>
   </si>
   <si>
     <t>A07:2021-Fallas de Identificación y Autenticación</t>
   </si>
   <si>
-    <t>A08:2021-Fallas en el Software y en la Integridad de los Datos</t>
-  </si>
-  <si>
-    <t>A09:2021-Fallos de Monitoreo y Registros de Seguridad*</t>
-  </si>
-  <si>
-    <t>A10:2021-Falsificación de solicitudes del lado del servidor (SSRF)*</t>
+    <t>A02:2021-Fallas Criptográficas</t>
+  </si>
+  <si>
+    <t>A05:2021-Configuración de Seguridad Incorrecta</t>
+  </si>
+  <si>
+    <t>A06:2021-Componentes Vulnerables y Desactualizados</t>
+  </si>
+  <si>
+    <t>A08:2021-Fallas en la Integridad del Software y de los Datos</t>
+  </si>
+  <si>
+    <t>A09:2021-Fallas en el Registro y Monitoreo de la Seguridad*</t>
+  </si>
+  <si>
+    <t>A10:2021-Falsificación de Solicitudes del Lado del Servidor (SSRF)*</t>
   </si>
 </sst>
 </file>
@@ -1197,8 +1197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26A41B76-54DA-6647-B3B3-A14FC0190F46}">
   <dimension ref="C6:E17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1248,7 +1248,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.2">
@@ -1257,7 +1257,7 @@
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="3:5" x14ac:dyDescent="0.2">
@@ -1265,7 +1265,7 @@
         <v>7</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.2">
@@ -1273,7 +1273,7 @@
         <v>8</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fix mapping Excel and image
</commit_message>
<xml_diff>
--- a/2021/docs/es/assets/Top10Mapping-es.xlsx
+++ b/2021/docs/es/assets/Top10Mapping-es.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinmarsicano/Git/OWASP/Top10/2021/docs/es/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164BF1B9-FBB5-1649-843D-266001A78B0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A458C9DF-FA1C-A049-BECE-D416326EFF11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6080" yWindow="-21100" windowWidth="25600" windowHeight="21100" xr2:uid="{C7D86A64-EE22-7643-AE64-D299E066CB54}"/>
+    <workbookView xWindow="19500" yWindow="-21100" windowWidth="25600" windowHeight="21100" xr2:uid="{C7D86A64-EE22-7643-AE64-D299E066CB54}"/>
   </bookViews>
   <sheets>
     <sheet name="Top 10 Mapping" sheetId="1" r:id="rId1"/>
@@ -36,61 +36,61 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
-    <t>(Nuevo)</t>
-  </si>
-  <si>
-    <t>* A partir de la encuesta</t>
-  </si>
-  <si>
-    <t>A01:2017-Inyección</t>
-  </si>
-  <si>
-    <t>A02:2017-Pérdida de Autenticación y Gestión de Sesiones</t>
-  </si>
-  <si>
-    <t>A03:2017-Exposición de Datos Sensibles</t>
-  </si>
-  <si>
-    <t>A04:2017-Entidad Externa de XML (XXE)</t>
-  </si>
-  <si>
-    <t>A05:2017-Pérdida de Control de Acceso</t>
-  </si>
-  <si>
-    <t>A06:2017-Configuración de Seguridad Incorrecta</t>
-  </si>
-  <si>
-    <t>A07:2017-Secuencia de Coamndos en Sitios Cruzados (XSS)</t>
-  </si>
-  <si>
-    <t>A08:2017-Deserialización Insegura</t>
-  </si>
-  <si>
-    <t>A09:2017-Uso de Componentes con Vulnerabilidades Conocidas</t>
-  </si>
-  <si>
-    <t>A10:2017-Registro y Monitoreo Insuficiente</t>
+    <t>A01:2017-Injection</t>
+  </si>
+  <si>
+    <t>A02:2017-Broken Authentication</t>
+  </si>
+  <si>
+    <t>A03:2017-Sensitive Data Exposure</t>
+  </si>
+  <si>
+    <t>A04:2017-XML External Entities (XXE)</t>
+  </si>
+  <si>
+    <t>(New)</t>
+  </si>
+  <si>
+    <t>A05:2017-Broken Access Control</t>
+  </si>
+  <si>
+    <t>A06:2017-Security Misconfiguration</t>
+  </si>
+  <si>
+    <t>A07:2017-Cross-Site Scripting (XSS)</t>
+  </si>
+  <si>
+    <t>A08:2017-Insecure Deserialization</t>
+  </si>
+  <si>
+    <t>A09:2017-Using Components with Known Vulnerabilities</t>
+  </si>
+  <si>
+    <t>A10:2017-Insufficient Logging &amp; Monitoring</t>
+  </si>
+  <si>
+    <t>* From the Survey</t>
   </si>
   <si>
     <t>A01:2021-Pérdida de Control de Acceso</t>
   </si>
   <si>
+    <t>A02:2021-Fallas Criptográficas</t>
+  </si>
+  <si>
     <t>A03:2021-Inyección</t>
   </si>
   <si>
-    <t>A06:2021-Componentes Vulnerables y Obsoletos</t>
+    <t>A04:2021-Diseño Inseguro</t>
+  </si>
+  <si>
+    <t>A05:2021-Configuración de Seguridad Incorrecta</t>
+  </si>
+  <si>
+    <t>A06:2021-Componentes Vulnerables y Desactualizados</t>
   </si>
   <si>
     <t>A07:2021-Fallas de Identificación y Autenticación</t>
-  </si>
-  <si>
-    <t>A02:2021-Fallas Criptográficas</t>
-  </si>
-  <si>
-    <t>A05:2021-Configuración de Seguridad Incorrecta</t>
-  </si>
-  <si>
-    <t>A06:2021-Componentes Vulnerables y Desactualizados</t>
   </si>
   <si>
     <t>A08:2021-Fallas en la Integridad del Software y de los Datos</t>
@@ -761,114 +761,6 @@
         <a:xfrm flipV="1">
           <a:off x="27368500" y="7424058"/>
           <a:ext cx="1574800" cy="187477"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:headEnd type="none" w="med" len="med"/>
-          <a:tailEnd type="arrow" w="med" len="med"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="accent6"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent6"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent6"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>110068</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>16933</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>99785</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="12" name="Straight Arrow Connector 11">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F9E0D9D-AF10-0448-90B8-FC5BA55B2BAD}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="5359400" y="2954868"/>
-          <a:ext cx="846666" cy="192917"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:headEnd type="none" w="med" len="med"/>
-          <a:tailEnd type="arrow" w="med" len="med"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="accent6"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent6"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent6"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>110068</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>16933</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>99785</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43A1CAA8-9EF5-934C-BC91-F93F7FCF516B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="5359400" y="2954868"/>
-          <a:ext cx="846666" cy="192917"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1197,14 +1089,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26A41B76-54DA-6647-B3B3-A14FC0190F46}">
   <dimension ref="C6:E17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="8" customWidth="1"/>
-    <col min="3" max="3" width="54.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="44.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1218,7 +1109,7 @@
     </row>
     <row r="7" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C7" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>12</v>
@@ -1226,62 +1117,62 @@
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C8" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C9" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C10" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C11" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C12" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C13" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C14" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>19</v>
@@ -1289,7 +1180,7 @@
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C15" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>20</v>
@@ -1297,10 +1188,10 @@
     </row>
     <row r="16" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C16" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>21</v>
@@ -1308,7 +1199,7 @@
     </row>
     <row r="17" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E17" s="7" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>